<commit_message>
a big one pre preso
</commit_message>
<xml_diff>
--- a/Workbook1.xlsx
+++ b/Workbook1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="11200" yWindow="3200" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,8 +151,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -180,20 +184,256 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power law index (aprox)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-7.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2142721448"/>
+        <c:axId val="-2142399064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2142721448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Radius of Interest</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142399064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2142399064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Power law index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142721448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" activeCellId="1" sqref="A1:A7 E1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -557,14 +797,14 @@
         <v>800</v>
       </c>
       <c r="D2" s="4">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="E2" s="4">
-        <v>-7.8</v>
+        <v>-7.1</v>
       </c>
       <c r="F2">
         <f>A2-(D2-(A2-B2))/2</f>
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" thickBot="1">
@@ -578,73 +818,98 @@
         <v>900</v>
       </c>
       <c r="D3" s="4">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E3" s="4">
-        <v>-7</v>
+        <v>-6.7</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F18" si="0">A3-(D3-(A3-B3))/2</f>
-        <v>143.5</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" thickBot="1">
       <c r="A4" s="3">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="B4" s="4">
         <v>80</v>
       </c>
       <c r="C4" s="4">
-        <v>1400</v>
+        <v>900</v>
       </c>
       <c r="D4" s="4">
-        <v>422</v>
+        <v>340</v>
       </c>
       <c r="E4" s="4">
-        <v>-6.5</v>
+        <v>-6.3</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>349</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" thickBot="1">
       <c r="A5" s="3">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="B5" s="4">
         <v>80</v>
       </c>
       <c r="C5" s="4">
+        <v>1300</v>
+      </c>
+      <c r="D5" s="4">
+        <v>440</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-5.8</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" thickBot="1">
+      <c r="A6" s="3">
+        <v>800</v>
+      </c>
+      <c r="B6" s="4">
+        <v>80</v>
+      </c>
+      <c r="C6" s="4">
         <v>2400</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>837</v>
       </c>
-      <c r="E5" s="4">
-        <v>-6</v>
-      </c>
-      <c r="F5">
+      <c r="E6" s="4">
+        <v>-5.7</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>741.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" thickBot="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="16" thickBot="1">
+      <c r="A7" s="3">
+        <v>1600</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1580</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4000</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3150</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-4</v>
+      </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -788,6 +1053,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>